<commit_message>
added deviance explained (not sure if the formula is actually right)
</commit_message>
<xml_diff>
--- a/boosted regression trees 08-06-2014.xlsx
+++ b/boosted regression trees 08-06-2014.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="28">
   <si>
     <t>FP richness</t>
   </si>
@@ -113,12 +113,21 @@
   <si>
     <t>VARIABLES</t>
   </si>
+  <si>
+    <t>% Deviance Explained</t>
+  </si>
+  <si>
+    <t>(Dev.null - Dev.resid) / Dev.null * 100</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -144,6 +153,13 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -195,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -211,6 +227,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,10 +537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F119"/>
+  <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -678,72 +703,66 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A20" s="11"/>
+      <c r="B20" s="8"/>
+    </row>
+    <row r="21" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="13">
+        <f>(B18-B19)/B18*100</f>
+        <v>39.311054631987687</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="4">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" s="4">
-        <v>0.18</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C24" s="4">
-        <v>0.14000000000000001</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C25" s="4">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C26" s="4">
-        <v>0.02</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -751,15 +770,15 @@
         <v>4</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C27" s="4">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>5</v>
@@ -770,727 +789,797 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="4">
+      <c r="B31" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="4">
         <v>0.01</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="6" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B36" s="4">
         <v>27.072793690000001</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B35" s="4">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="4">
         <v>14.43483054</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B38" s="4">
         <v>11.018921479999999</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B39" s="4">
         <v>10.165041459999999</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B38" s="4">
+      <c r="B40" s="4">
         <v>9.2858573100000008</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="4">
+      <c r="B41" s="4">
         <v>6.2823325499999996</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B40" s="4">
+      <c r="B42" s="4">
         <v>5.5913260999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B41" s="4">
+      <c r="B43" s="4">
         <v>4.48070754</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B42" s="4">
+      <c r="B44" s="4">
         <v>4.3034100899999999</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B43" s="4">
+      <c r="B45" s="4">
         <v>3.8307832500000001</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B44" s="4">
+      <c r="B46" s="4">
         <v>2.09210831</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B45" s="4">
+      <c r="B47" s="4">
         <v>1.4184818800000001</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="4" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B46" s="4">
+      <c r="B48" s="4">
         <v>2.3405809999999999E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="5" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B48" s="4">
+      <c r="B50" s="4">
         <v>218.63030000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="5" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B49" s="4">
+      <c r="B51" s="4">
         <v>144.35499999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="2"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="11"/>
+      <c r="B52" s="8"/>
+    </row>
+    <row r="53" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C53" s="13">
+        <f>(B50-B51)/B50*100</f>
+        <v>33.973012889796159</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="2"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C52" s="4">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C53" s="4">
-        <v>0.53</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C54" s="4">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C55" s="4">
-        <v>0.23</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C56" s="4">
-        <v>0.14000000000000001</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C57" s="4">
-        <v>0.11</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C58" s="4">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="4">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B60" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" s="4">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C61" s="4">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C59" s="4">
+      <c r="C63" s="4">
         <v>0.09</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="6" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B67" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B64" s="4">
+      <c r="B68" s="4">
         <v>19.162904770000001</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A65" s="4" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B65" s="4">
+      <c r="B69" s="4">
         <v>16.637263440000002</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B66" s="4">
+      <c r="B70" s="4">
         <v>12.969857080000001</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B67" s="4">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B71" s="4">
         <v>11.680253990000001</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="4" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="4">
+      <c r="B72" s="4">
         <v>8.0937943200000007</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="4" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B69" s="4">
+      <c r="B73" s="4">
         <v>8.0513572900000003</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="4" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B70" s="4">
+      <c r="B74" s="4">
         <v>6.2434783200000004</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B71" s="4">
+      <c r="B75" s="4">
         <v>5.9796862700000002</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" s="4" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B72" s="4">
+      <c r="B76" s="4">
         <v>4.1156138499999999</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="4" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B73" s="4">
+      <c r="B77" s="4">
         <v>3.7446742300000002</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="4" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B74" s="4">
+      <c r="B78" s="4">
         <v>2.26016255</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" s="4" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B75" s="4">
+      <c r="B79" s="4">
         <v>0.98920014000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" s="4" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B76" s="4">
+      <c r="B80" s="4">
         <v>7.1753739999999996E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" s="5" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B78" s="4">
+      <c r="B82" s="4">
         <v>163.07050000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" s="5" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B79" s="4">
+      <c r="B83" s="4">
         <v>118.60980000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" s="2"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="3" t="s">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="11"/>
+      <c r="B84" s="8"/>
+    </row>
+    <row r="85" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A85" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B85" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C85" s="13">
+        <f>(B82-B83)/B82*100</f>
+        <v>27.264710661952957</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="2"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B87" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="C87" s="3" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C82" s="4">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C83" s="4">
-        <v>0.28999999999999998</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C84" s="4">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C85" s="4">
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C86" s="4">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C87" s="4">
-        <v>0.11</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C88" s="4">
-        <v>0.1</v>
+        <v>0.37</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C89" s="4">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C90" s="4">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C91" s="4">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B89" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C89" s="4">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B91" s="7"/>
-      <c r="C91" s="7"/>
+      <c r="B92" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C92" s="4">
+        <v>0.16</v>
+      </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>17</v>
+      <c r="A93" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C93" s="4">
+        <v>0.11</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B94" s="4">
-        <v>25.374683099999999</v>
+        <v>22</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="4">
+        <v>0.1</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B95" s="4">
-        <v>18.816661199999999</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B96" s="4">
-        <v>9.9158559999999998</v>
+      <c r="B95" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C95" s="4">
+        <v>0.08</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B97" s="4">
-        <v>9.6778879</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B98" s="4">
-        <v>7.1040961999999999</v>
-      </c>
+      <c r="A97" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B97" s="7"/>
+      <c r="C97" s="7"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B99" s="4">
-        <v>6.5019108000000001</v>
+      <c r="A99" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B100" s="4">
-        <v>5.9024751999999996</v>
+        <v>25.374683099999999</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B101" s="4">
-        <v>4.9036923000000003</v>
+        <v>18.816661199999999</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B102" s="4">
-        <v>3.930688</v>
+        <v>9.9158559999999998</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B103" s="4">
-        <v>3.8076219</v>
+        <v>9.6778879</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B104" s="4">
-        <v>2.2710181</v>
+        <v>7.1040961999999999</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B105" s="4">
-        <v>1.4817947</v>
+        <v>6.5019108000000001</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B106" s="4">
-        <v>0.31161460000000002</v>
+        <v>5.9024751999999996</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B107" s="4">
+        <v>4.9036923000000003</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A108" s="5" t="s">
-        <v>18</v>
+      <c r="A108" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="B108" s="4">
-        <v>135.9</v>
+        <v>3.930688</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A109" s="5" t="s">
-        <v>19</v>
+      <c r="A109" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="B109" s="4">
-        <v>90.812399999999997</v>
+        <v>3.8076219</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A110" s="2"/>
+      <c r="A110" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B110" s="4">
+        <v>2.2710181</v>
+      </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A111" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B111" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C111" s="3" t="s">
-        <v>15</v>
+      <c r="A111" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B111" s="4">
+        <v>1.4817947</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B112" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B112" s="4">
+        <v>0.31161460000000002</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B114" s="4">
+        <v>135.9</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B115" s="4">
+        <v>90.812399999999997</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" s="11"/>
+      <c r="B116" s="8"/>
+    </row>
+    <row r="117" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A117" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B117" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C117" s="13">
+        <f>(B114-B115)/B114*100</f>
+        <v>33.177041942604859</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" s="2"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B119" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B120" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C112" s="4">
+      <c r="C120" s="4">
         <v>1.38</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A113" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B113" s="4" t="s">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B121" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C113" s="4">
+      <c r="C121" s="4">
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A114" s="4" t="s">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B122" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C114" s="4">
+      <c r="C122" s="4">
         <v>0.44</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A115" s="4" t="s">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B123" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C115" s="4">
+      <c r="C123" s="4">
         <v>0.37</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A116" s="4" t="s">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B116" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C116" s="4">
+      <c r="B124" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C124" s="4">
         <v>0.27</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A117" s="4" t="s">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B117" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C117" s="4">
+      <c r="B125" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C125" s="4">
         <v>0.23</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A118" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B118" s="4" t="s">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B126" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C118" s="4">
+      <c r="C126" s="4">
         <v>0.21</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A119" s="4" t="s">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B127" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C119" s="4">
+      <c r="C127" s="4">
         <v>0.1</v>
       </c>
     </row>
@@ -1501,9 +1590,9 @@
     <oddFooter>&amp;C&amp;F</oddFooter>
   </headerFooter>
   <rowBreaks count="3" manualBreakCount="3">
-    <brk id="30" max="16383" man="1"/>
-    <brk id="60" max="16383" man="1"/>
-    <brk id="90" max="16383" man="1"/>
+    <brk id="32" max="16383" man="1"/>
+    <brk id="64" max="16383" man="1"/>
+    <brk id="96" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>